<commit_message>
finished qs1, 2, 3 / redo 4
</commit_message>
<xml_diff>
--- a/background/isp_util_var_list_20230209.xlsx
+++ b/background/isp_util_var_list_20230209.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\FHPC\DATA\HCPF_Data_files_SECURE\Kim\isp\isp_utilization\01_background\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\FHPC\DATA\HCPF_Data_files_SECURE\Kim\isp\isp_utilization\background\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9150C676-4C28-4992-9695-9EDCF49204B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32EA277D-A705-4FD1-80C5-A5143E46CDF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,10 +19,19 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">vars!$A$2:$M$57</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -63,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="229">
   <si>
     <t>Variable</t>
   </si>
@@ -800,9 +809,6 @@
     <t>indicator ISP : for mems, use DT_START_PRAC_ISP (row 15)</t>
   </si>
   <si>
-    <t>ind_ISP_prac</t>
-  </si>
-  <si>
     <t>ind_ISP_mem</t>
   </si>
   <si>
@@ -813,7 +819,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -981,6 +987,14 @@
       <name val="Albany AMT"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1035,7 +1049,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1144,6 +1158,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1467,13 +1484,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="I57" sqref="I57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.21875" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" customWidth="1"/>
     <col min="2" max="2" width="26.33203125" style="12" customWidth="1"/>
     <col min="3" max="3" width="7.21875" customWidth="1"/>
     <col min="4" max="4" width="13" style="12" customWidth="1"/>
@@ -1659,7 +1676,7 @@
         <v>46</v>
       </c>
       <c r="K6" s="1"/>
-      <c r="L6" s="17" t="s">
+      <c r="L6" s="45" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1699,7 +1716,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
@@ -1714,24 +1731,12 @@
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="10"/>
-      <c r="C9" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D9" s="30">
-        <v>1</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" s="1">
-        <v>8</v>
-      </c>
-      <c r="H9" s="43" t="s">
-        <v>226</v>
-      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="43"/>
       <c r="I9" s="1" t="s">
         <v>42</v>
       </c>
@@ -3073,10 +3078,10 @@
         <v>114</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="K56" s="3" t="s">
         <v>139</v>
@@ -3122,8 +3127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D983EC1-0949-4F06-91D1-4D369B6FAF1E}">
   <dimension ref="A1:B96"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>